<commit_message>
now includes flowrate in pipes etc
</commit_message>
<xml_diff>
--- a/trunk/EnFloSW/Manuals/FID/Determine Leak rate from change pressure drop.xlsx
+++ b/trunk/EnFloSW/Manuals/FID/Determine Leak rate from change pressure drop.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="22995" windowHeight="11310"/>
+    <workbookView xWindow="13305" yWindow="-15" windowWidth="13170" windowHeight="9870" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Calib gases" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
   <si>
     <t>P static</t>
   </si>
@@ -76,14 +76,130 @@
   </si>
   <si>
     <t>m^3</t>
+  </si>
+  <si>
+    <t>Q=AU</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>m^2</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>l/min</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>m^3/S</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Dynamic press</t>
+  </si>
+  <si>
+    <t>reduction in Area to get pressure rise</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>Propane</t>
+  </si>
+  <si>
+    <t>Velocity</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>N/m2</t>
+  </si>
+  <si>
+    <t>mBar</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>voulme of pipe</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Litres</t>
+  </si>
+  <si>
+    <t>Carrier</t>
+  </si>
+  <si>
+    <t>Trace</t>
+  </si>
+  <si>
+    <t>Desired ppm</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Fixing the Trace Flowrate</t>
+  </si>
+  <si>
+    <t>Fixing the Carrier Flowrate</t>
+  </si>
+  <si>
+    <t>Use Carrier 2 50</t>
+  </si>
+  <si>
+    <t>Source</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -191,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -202,6 +318,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,14 +622,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L9"/>
+  <dimension ref="B1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -677,6 +797,167 @@
       <c r="L9" s="9">
         <f>(C9/B9)*K9</f>
         <v>0.24009293920232086</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" t="s">
+        <v>34</v>
+      </c>
+      <c r="J23" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" t="s">
+        <v>40</v>
+      </c>
+      <c r="J24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>1.4</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <f>PI()*(C26/1000)^2/4</f>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="E26">
+        <f>B26/60000</f>
+        <v>2.3333333333333332E-5</v>
+      </c>
+      <c r="F26">
+        <f>E26/D26</f>
+        <v>7.4272306776217822E-2</v>
+      </c>
+      <c r="H26">
+        <v>7</v>
+      </c>
+      <c r="I26">
+        <v>2.012</v>
+      </c>
+      <c r="J26">
+        <f>0.5*I26*H26^2</f>
+        <v>49.293999999999997</v>
+      </c>
+      <c r="K26">
+        <f>J26/100</f>
+        <v>0.49293999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <f>25.4*0.012</f>
+        <v>0.30480000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>20</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="D39">
+        <f>PI()*(B39/1000)^2/4</f>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="E39">
+        <f>D39*1000</f>
+        <v>0.31415926535897931</v>
       </c>
     </row>
   </sheetData>
@@ -686,13 +967,400 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X23" sqref="X23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" t="s">
+        <v>45</v>
+      </c>
+      <c r="O7" t="s">
+        <v>49</v>
+      </c>
+      <c r="P7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" t="s">
+        <v>46</v>
+      </c>
+      <c r="P8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N9" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>300</v>
+      </c>
+      <c r="E11" s="12">
+        <v>50</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" ref="F11:F17" si="0">E11/A$3</f>
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:G17" si="1">E11*D11/1000000</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H11" s="10">
+        <f t="shared" ref="H11:H17" si="2">G11/B$3</f>
+        <v>0.3</v>
+      </c>
+      <c r="L11">
+        <v>300</v>
+      </c>
+      <c r="M11" s="11">
+        <f>1000000*O11/L11</f>
+        <v>50</v>
+      </c>
+      <c r="N11" s="10">
+        <f>M11/A$3</f>
+        <v>1</v>
+      </c>
+      <c r="O11" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P11" s="10">
+        <f>O11/B$3</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>600</v>
+      </c>
+      <c r="E12" s="12">
+        <v>25</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H12" s="10">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="L12">
+        <v>600</v>
+      </c>
+      <c r="M12" s="11">
+        <f t="shared" ref="M12:M14" si="3">1000000*O12/L12</f>
+        <v>25</v>
+      </c>
+      <c r="N12" s="10">
+        <f>M12/A$3</f>
+        <v>0.5</v>
+      </c>
+      <c r="O12" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P12" s="10">
+        <f>O12/B$3</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>900</v>
+      </c>
+      <c r="E13" s="12">
+        <v>50</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="H13" s="10">
+        <f t="shared" si="2"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="L13">
+        <v>900</v>
+      </c>
+      <c r="M13" s="11">
+        <f t="shared" si="3"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="N13" s="10">
+        <f>M13/A$3</f>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="O13" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P13" s="10">
+        <f>O13/B$3</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>800</v>
+      </c>
+      <c r="E14" s="12">
+        <v>5</v>
+      </c>
+      <c r="F14" s="10">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H14" s="10">
+        <f t="shared" si="2"/>
+        <v>0.08</v>
+      </c>
+      <c r="L14">
+        <v>400</v>
+      </c>
+      <c r="M14" s="11">
+        <f t="shared" si="3"/>
+        <v>37.5</v>
+      </c>
+      <c r="N14" s="10">
+        <f>M14/A$3</f>
+        <v>0.75</v>
+      </c>
+      <c r="O14" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P14" s="10">
+        <f>O14/B$3</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>1000</v>
+      </c>
+      <c r="E15" s="12">
+        <v>5</v>
+      </c>
+      <c r="F15" s="10">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H15" s="10">
+        <f t="shared" si="2"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="L15">
+        <v>400</v>
+      </c>
+      <c r="M15" s="11">
+        <f t="shared" ref="M15" si="4">1000000*O15/L15</f>
+        <v>37.5</v>
+      </c>
+      <c r="N15" s="10">
+        <f>M15/A$3</f>
+        <v>0.75</v>
+      </c>
+      <c r="O15" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P15" s="10">
+        <f>O15/B$3</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>10000</v>
+      </c>
+      <c r="E16" s="12">
+        <v>5</v>
+      </c>
+      <c r="F16" s="10">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>400</v>
+      </c>
+      <c r="M16" s="11">
+        <f t="shared" ref="M16:M17" si="5">1000000*O16/L16</f>
+        <v>37.5</v>
+      </c>
+      <c r="N16" s="10">
+        <f>M16/A$3</f>
+        <v>0.75</v>
+      </c>
+      <c r="O16" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P16" s="10">
+        <f>O16/B$3</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>20000</v>
+      </c>
+      <c r="E17" s="12">
+        <v>1.4</v>
+      </c>
+      <c r="F17" s="10">
+        <f t="shared" si="0"/>
+        <v>2.7999999999999997E-2</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" si="2"/>
+        <v>0.55999999999999994</v>
+      </c>
+      <c r="L17">
+        <v>20000</v>
+      </c>
+      <c r="M17" s="11">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N17" s="10">
+        <f>M17/A$3</f>
+        <v>0.02</v>
+      </c>
+      <c r="O17" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="P17" s="10">
+        <f>O17/B$3</f>
+        <v>0.39999999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
now gives calculations of calibration carrier strength mixing
</commit_message>
<xml_diff>
--- a/trunk/EnFloSW/Manuals/FID/Determine Leak rate from change pressure drop.xlsx
+++ b/trunk/EnFloSW/Manuals/FID/Determine Leak rate from change pressure drop.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
   <si>
     <t>P static</t>
   </si>
@@ -181,6 +181,21 @@
   </si>
   <si>
     <t>Source</t>
+  </si>
+  <si>
+    <t>source gas</t>
+  </si>
+  <si>
+    <t>Calib ppm</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>Q total</t>
   </si>
 </sst>
 </file>
@@ -967,13 +982,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1109,14 +1127,14 @@
         <v>50</v>
       </c>
       <c r="N11" s="10">
-        <f>M11/A$3</f>
+        <f t="shared" ref="N11:N17" si="3">M11/A$3</f>
         <v>1</v>
       </c>
       <c r="O11" s="12">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="P11" s="10">
-        <f>O11/B$3</f>
+        <f t="shared" ref="P11:P17" si="4">O11/B$3</f>
         <v>0.3</v>
       </c>
     </row>
@@ -1143,18 +1161,18 @@
         <v>600</v>
       </c>
       <c r="M12" s="11">
-        <f t="shared" ref="M12:M14" si="3">1000000*O12/L12</f>
+        <f t="shared" ref="M12:M14" si="5">1000000*O12/L12</f>
         <v>25</v>
       </c>
       <c r="N12" s="10">
-        <f>M12/A$3</f>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="O12" s="12">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="P12" s="10">
-        <f>O12/B$3</f>
+        <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
     </row>
@@ -1181,18 +1199,18 @@
         <v>900</v>
       </c>
       <c r="M13" s="11">
+        <f t="shared" si="5"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="N13" s="10">
         <f t="shared" si="3"/>
-        <v>16.666666666666668</v>
-      </c>
-      <c r="N13" s="10">
-        <f>M13/A$3</f>
         <v>0.33333333333333337</v>
       </c>
       <c r="O13" s="12">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="P13" s="10">
-        <f>O13/B$3</f>
+        <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
     </row>
@@ -1219,18 +1237,18 @@
         <v>400</v>
       </c>
       <c r="M14" s="11">
+        <f t="shared" si="5"/>
+        <v>37.5</v>
+      </c>
+      <c r="N14" s="10">
         <f t="shared" si="3"/>
-        <v>37.5</v>
-      </c>
-      <c r="N14" s="10">
-        <f>M14/A$3</f>
         <v>0.75</v>
       </c>
       <c r="O14" s="12">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="P14" s="10">
-        <f>O14/B$3</f>
+        <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
     </row>
@@ -1257,18 +1275,18 @@
         <v>400</v>
       </c>
       <c r="M15" s="11">
-        <f t="shared" ref="M15" si="4">1000000*O15/L15</f>
+        <f t="shared" ref="M15" si="6">1000000*O15/L15</f>
         <v>37.5</v>
       </c>
       <c r="N15" s="10">
-        <f>M15/A$3</f>
+        <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
       <c r="O15" s="12">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="P15" s="10">
-        <f>O15/B$3</f>
+        <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
     </row>
@@ -1295,18 +1313,18 @@
         <v>400</v>
       </c>
       <c r="M16" s="11">
-        <f t="shared" ref="M16:M17" si="5">1000000*O16/L16</f>
+        <f t="shared" ref="M16:M17" si="7">1000000*O16/L16</f>
         <v>37.5</v>
       </c>
       <c r="N16" s="10">
-        <f>M16/A$3</f>
+        <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
       <c r="O16" s="12">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="P16" s="10">
-        <f>O16/B$3</f>
+        <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
     </row>
@@ -1333,18 +1351,18 @@
         <v>20000</v>
       </c>
       <c r="M17" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N17" s="10">
-        <f>M17/A$3</f>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
       <c r="O17" s="12">
         <v>0.02</v>
       </c>
       <c r="P17" s="10">
-        <f>O17/B$3</f>
+        <f t="shared" si="4"/>
         <v>0.39999999999999997</v>
       </c>
     </row>
@@ -1356,6 +1374,102 @@
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" t="s">
+        <v>57</v>
+      </c>
+      <c r="J25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>1000</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>50</v>
+      </c>
+      <c r="H26">
+        <f>G26*F26/E26</f>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f>G26*(E26-F26)/E26</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>1000</v>
+      </c>
+      <c r="F27">
+        <v>250</v>
+      </c>
+      <c r="G27">
+        <v>50</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ref="H27:H30" si="8">G27*F27/E27</f>
+        <v>12.5</v>
+      </c>
+      <c r="I27">
+        <f t="shared" ref="I27:I30" si="9">G27*(E27-F27)/E27</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>1000</v>
+      </c>
+      <c r="F28">
+        <v>500</v>
+      </c>
+      <c r="G28">
+        <v>50</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>1000</v>
+      </c>
+      <c r="F29">
+        <v>750</v>
+      </c>
+      <c r="G29">
+        <v>50</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="8"/>
+        <v>37.5</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="9"/>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Recent tweaks on the EnFlo Tunnel Machine
</commit_message>
<xml_diff>
--- a/trunk/EnFloSW/Manuals/FID/Determine Leak rate from change pressure drop.xlsx
+++ b/trunk/EnFloSW/Manuals/FID/Determine Leak rate from change pressure drop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="13305" yWindow="-15" windowWidth="13170" windowHeight="9870" activeTab="1"/>
+    <workbookView xWindow="13305" yWindow="-15" windowWidth="13170" windowHeight="9870"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,22 +891,22 @@
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="C26">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D26">
         <f>PI()*(C26/1000)^2/4</f>
-        <v>3.1415926535897931E-4</v>
+        <v>1.2566370614359172E-5</v>
       </c>
       <c r="E26">
         <f>B26/60000</f>
-        <v>2.3333333333333332E-5</v>
+        <v>3.3333333333333335E-5</v>
       </c>
       <c r="F26">
         <f>E26/D26</f>
-        <v>7.4272306776217822E-2</v>
+        <v>2.6525823848649228</v>
       </c>
       <c r="H26">
         <v>7</v>
@@ -984,7 +984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
@@ -1426,11 +1426,11 @@
         <v>50</v>
       </c>
       <c r="H27">
-        <f t="shared" ref="H27:H30" si="8">G27*F27/E27</f>
+        <f t="shared" ref="H27:H29" si="8">G27*F27/E27</f>
         <v>12.5</v>
       </c>
       <c r="I27">
-        <f t="shared" ref="I27:I30" si="9">G27*(E27-F27)/E27</f>
+        <f t="shared" ref="I27:I29" si="9">G27*(E27-F27)/E27</f>
         <v>37.5</v>
       </c>
     </row>

</xml_diff>